<commit_message>
Rigtig inv og insignifikant eksport P
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonaselkjaer/Library/CloudStorage/OneDrive-Personligt/Uni/4. Semester/Projekt/projekt4sem/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_AD4D1D646341095ACB70006885D5DC46683EDF11" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5072446-38B9-C24D-8C55-58EEB268E65E}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="113_{CDC0F0DD-205A-2044-ACD8-BEB3E9E52EAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC9A0DAB-72BF-7F46-9324-93C2B6C6206B}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="2460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -448,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -565,14 +565,14 @@
         <v>0.53898548126904466</v>
       </c>
       <c r="D2" s="3" t="e">
-        <f>Q2/I2</f>
+        <f t="shared" ref="D2:D33" si="1">Q2/I2</f>
         <v>#VALUE!</v>
       </c>
       <c r="E2" s="3">
         <v>64.3</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F33" si="1">100-E2</f>
+        <f t="shared" ref="F2:F33" si="2">100-E2</f>
         <v>35.700000000000003</v>
       </c>
       <c r="G2" s="3">
@@ -593,7 +593,7 @@
         <v>10918265962035.9</v>
       </c>
       <c r="L2" s="5">
-        <f>K2-I2/X2</f>
+        <f t="shared" ref="L2:L33" si="3">K2-I2/X2</f>
         <v>10918265961955.129</v>
       </c>
       <c r="M2" s="1">
@@ -606,11 +606,11 @@
         <v>24</v>
       </c>
       <c r="P2" s="3" t="e">
-        <f t="shared" ref="P2:P33" si="2">O2/N2</f>
+        <f t="shared" ref="P2:P33" si="4">O2/N2</f>
         <v>#VALUE!</v>
       </c>
       <c r="Q2" s="3" t="e">
-        <f t="shared" ref="Q2:Q33" si="3">P2*M2</f>
+        <f t="shared" ref="Q2:Q33" si="5">P2*M2</f>
         <v>#VALUE!</v>
       </c>
       <c r="R2" s="1"/>
@@ -629,7 +629,7 @@
         <v>4.5064169205950889E-2</v>
       </c>
       <c r="Z2" s="3">
-        <f t="shared" ref="Z2:Z33" si="4">Y2*S2</f>
+        <f t="shared" ref="Z2:Z64" si="6">Y2*S2</f>
         <v>0.35600693672701206</v>
       </c>
       <c r="AA2" s="6">
@@ -652,22 +652,22 @@
         <v>0.5437236731255265</v>
       </c>
       <c r="D3" s="3" t="e">
-        <f>Q3/I3</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="E3" s="3">
         <v>65.2</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34.799999999999997</v>
       </c>
       <c r="G3" s="3">
-        <f t="shared" ref="G3:G64" si="5">E3/100*AA3</f>
+        <f t="shared" ref="G3:G64" si="7">E3/100*AA3</f>
         <v>351.44390243902438</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H64" si="6">F3/100*AA3</f>
+        <f t="shared" ref="H3:H64" si="8">F3/100*AA3</f>
         <v>187.58048780487803</v>
       </c>
       <c r="I3" s="3">
@@ -680,7 +680,7 @@
         <v>11330203833282.875</v>
       </c>
       <c r="L3" s="5">
-        <f>K3-I3/X3</f>
+        <f t="shared" si="3"/>
         <v>11330203833196.949</v>
       </c>
       <c r="M3" s="1">
@@ -693,11 +693,11 @@
         <v>24</v>
       </c>
       <c r="P3" s="3" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="Q3" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="R3" s="1">
@@ -714,15 +714,15 @@
         <v>6.9071400059071397</v>
       </c>
       <c r="Y3" s="2">
-        <f>E3/100*(J3/I3)</f>
+        <f t="shared" ref="Y3:Y64" si="9">E3/100*(J3/I3)</f>
         <v>4.8556697556866056E-2</v>
       </c>
       <c r="Z3" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.39816491996630171</v>
       </c>
       <c r="AA3" s="6">
-        <f t="shared" ref="AA3:AA64" si="7">J3/S3*100</f>
+        <f t="shared" ref="AA3:AA64" si="10">J3/S3*100</f>
         <v>539.02439024390242</v>
       </c>
       <c r="AB3" s="4">
@@ -741,22 +741,22 @@
         <v>0.5450486365810876</v>
       </c>
       <c r="D4" s="3" t="e">
-        <f>Q4/I4</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="E4" s="3">
         <v>65.8</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34.200000000000003</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>370.12499999999989</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>192.37499999999997</v>
       </c>
       <c r="I4" s="3">
@@ -769,7 +769,7 @@
         <v>11939243133605.314</v>
       </c>
       <c r="L4" s="5">
-        <f>K4-I4/X4</f>
+        <f t="shared" si="3"/>
         <v>11939243133514.523</v>
       </c>
       <c r="M4" s="1">
@@ -782,11 +782,11 @@
         <v>24</v>
       </c>
       <c r="P4" s="3" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="Q4" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="R4" s="1">
@@ -803,15 +803,15 @@
         <v>6.9071400059071397</v>
       </c>
       <c r="Y4" s="2">
-        <f>E4/100*(J4/I4)</f>
+        <f t="shared" si="9"/>
         <v>5.1939084675490348E-2</v>
       </c>
       <c r="Z4" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.45706394514431509</v>
       </c>
       <c r="AA4" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>562.49999999999989</v>
       </c>
       <c r="AB4" s="4">
@@ -830,22 +830,22 @@
         <v>0.54175249564252903</v>
       </c>
       <c r="D5" s="3" t="e">
-        <f>Q5/I5</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="E5" s="3">
         <v>66.100000000000009</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33.899999999999991</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>370.30215053763436</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>189.91290322580639</v>
       </c>
       <c r="I5" s="3">
@@ -858,7 +858,7 @@
         <v>12559478145397.666</v>
       </c>
       <c r="L5" s="5">
-        <f>K5-I5/X5</f>
+        <f t="shared" si="3"/>
         <v>12559478145306.297</v>
       </c>
       <c r="M5" s="1">
@@ -871,11 +871,11 @@
         <v>24</v>
       </c>
       <c r="P5" s="3" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="Q5" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="R5" s="1">
@@ -892,15 +892,15 @@
         <v>6.9071400059071397</v>
       </c>
       <c r="Y5" s="2">
-        <f>E5/100*(J5/I5)</f>
+        <f t="shared" si="9"/>
         <v>5.4568372682617647E-2</v>
       </c>
       <c r="Z5" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.50748586594834411</v>
       </c>
       <c r="AA5" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>560.21505376344078</v>
       </c>
       <c r="AB5" s="4">
@@ -919,22 +919,22 @@
         <v>0.53465777262180969</v>
       </c>
       <c r="D6" s="3" t="e">
-        <f>Q6/I6</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="E6" s="3">
         <v>65.400000000000006</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34.599999999999994</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>401.16494845360819</v>
       </c>
       <c r="H6" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>212.23711340206177</v>
       </c>
       <c r="I6" s="3">
@@ -947,7 +947,7 @@
         <v>13383942060792.504</v>
       </c>
       <c r="L6" s="5">
-        <f>K6-I6/X6</f>
+        <f t="shared" si="3"/>
         <v>13383942060692.666</v>
       </c>
       <c r="M6" s="1">
@@ -960,11 +960,11 @@
         <v>24</v>
       </c>
       <c r="P6" s="3" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="Q6" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="R6" s="1">
@@ -981,15 +981,15 @@
         <v>6.9071400059071397</v>
       </c>
       <c r="Y6" s="2">
-        <f>E6/100*(J6/I6)</f>
+        <f t="shared" si="9"/>
         <v>5.6428364269141537E-2</v>
       </c>
       <c r="Z6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.54735513341067299</v>
       </c>
       <c r="AA6" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>613.40206185567001</v>
       </c>
       <c r="AB6" s="4">
@@ -1008,22 +1008,22 @@
         <v>0.52898751733703198</v>
       </c>
       <c r="D7" s="3" t="e">
-        <f>Q7/I7</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="E7" s="3">
         <v>67.900000000000006</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32.099999999999994</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>433.51538461538462</v>
       </c>
       <c r="H7" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>204.94615384615381</v>
       </c>
       <c r="I7" s="3">
@@ -1036,7 +1036,7 @@
         <v>14130424920432.734</v>
       </c>
       <c r="L7" s="5">
-        <f>K7-I7/X7</f>
+        <f t="shared" si="3"/>
         <v>14130424920328.35</v>
       </c>
       <c r="M7" s="1">
@@ -1049,11 +1049,11 @@
         <v>24</v>
       </c>
       <c r="P7" s="3" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="Q7" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="R7" s="1">
@@ -1070,15 +1070,15 @@
         <v>6.9071400059071397</v>
       </c>
       <c r="Y7" s="2">
-        <f>E7/100*(J7/I7)</f>
+        <f t="shared" si="9"/>
         <v>6.2532038834951467E-2</v>
       </c>
       <c r="Z7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.65033320388349525</v>
       </c>
       <c r="AA7" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>638.46153846153845</v>
       </c>
       <c r="AB7" s="4">
@@ -1097,22 +1097,22 @@
         <v>0.53685205183585294</v>
       </c>
       <c r="D8" s="3" t="e">
-        <f>Q8/I8</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="E8" s="3">
         <v>69</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>450.05405405405406</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>202.19819819819821</v>
       </c>
       <c r="I8" s="3">
@@ -1125,7 +1125,7 @@
         <v>14941564574955.998</v>
       </c>
       <c r="L8" s="5">
-        <f>K8-I8/X8</f>
+        <f t="shared" si="3"/>
         <v>14941564574848.746</v>
       </c>
       <c r="M8" s="1">
@@ -1138,11 +1138,11 @@
         <v>24</v>
       </c>
       <c r="P8" s="3" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="Q8" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="R8" s="1">
@@ -1159,15 +1159,15 @@
         <v>6.9071400059071397</v>
       </c>
       <c r="Y8" s="2">
-        <f>E8/100*(J8/I8)</f>
+        <f t="shared" si="9"/>
         <v>6.7435205183585298E-2</v>
       </c>
       <c r="Z8" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.74853077753779673</v>
       </c>
       <c r="AA8" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>652.25225225225233</v>
       </c>
       <c r="AB8" s="4">
@@ -1186,22 +1186,22 @@
         <v>0.54284983371706319</v>
       </c>
       <c r="D9" s="3" t="e">
-        <f>Q9/I9</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="E9" s="3">
         <v>69.8</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30.200000000000003</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>477.16724137931044</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>206.45344827586214</v>
       </c>
       <c r="I9" s="3">
@@ -1214,7 +1214,7 @@
         <v>15557762218622.252</v>
       </c>
       <c r="L9" s="5">
-        <f>K9-I9/X9</f>
+        <f t="shared" si="3"/>
         <v>15557762218509.869</v>
       </c>
       <c r="M9" s="1">
@@ -1227,11 +1227,11 @@
         <v>24</v>
       </c>
       <c r="P9" s="3" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="Q9" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="R9" s="1">
@@ -1256,15 +1256,15 @@
         <v>6.9565416720476199</v>
       </c>
       <c r="Y9" s="2">
-        <f>E9/100*(J9/I9)</f>
+        <f t="shared" si="9"/>
         <v>7.0799948836019436E-2</v>
       </c>
       <c r="Z9" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.82127940649782538</v>
       </c>
       <c r="AA9" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>683.62068965517255</v>
       </c>
       <c r="AB9" s="4">
@@ -1283,22 +1283,22 @@
         <v>0.53284052350945221</v>
       </c>
       <c r="D10" s="3" t="e">
-        <f>Q10/I10</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="E10" s="3">
         <v>70</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>497.39837398373976</v>
       </c>
       <c r="H10" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>213.17073170731706</v>
       </c>
       <c r="I10" s="3">
@@ -1311,7 +1311,7 @@
         <v>16479035744545.393</v>
       </c>
       <c r="L10" s="5">
-        <f>K10-I10/X10</f>
+        <f t="shared" si="3"/>
         <v>16479035744435.365</v>
       </c>
       <c r="M10" s="1">
@@ -1324,11 +1324,11 @@
         <v>24</v>
       </c>
       <c r="P10" s="3" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="Q10" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="R10" s="1">
@@ -1353,15 +1353,15 @@
         <v>7.5000000064999996</v>
       </c>
       <c r="Y10" s="2">
-        <f>E10/100*(J10/I10)</f>
+        <f t="shared" si="9"/>
         <v>7.4139602520601061E-2</v>
       </c>
       <c r="Z10" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.91191711100339312</v>
       </c>
       <c r="AA10" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>710.56910569105685</v>
       </c>
       <c r="AB10" s="4">
@@ -1380,22 +1380,22 @@
         <v>0.52884287177153255</v>
       </c>
       <c r="D11" s="3" t="e">
-        <f>Q11/I11</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="E11" s="3">
         <v>69.400000000000006</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30.599999999999994</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>525.23181818181831</v>
       </c>
       <c r="H11" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>231.58636363636361</v>
       </c>
       <c r="I11" s="3">
@@ -1408,7 +1408,7 @@
         <v>17432951913806.617</v>
       </c>
       <c r="L11" s="5">
-        <f>K11-I11/X11</f>
+        <f t="shared" si="3"/>
         <v>17432951913689.43</v>
       </c>
       <c r="M11" s="1">
@@ -1421,11 +1421,11 @@
         <v>24</v>
       </c>
       <c r="P11" s="3" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="Q11" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="R11" s="1">
@@ -1450,15 +1450,15 @@
         <v>7.5000000064999996</v>
       </c>
       <c r="Y11" s="2">
-        <f>E11/100*(J11/I11)</f>
+        <f t="shared" si="9"/>
         <v>7.8883376948458303E-2</v>
       </c>
       <c r="Z11" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0412605757196496</v>
       </c>
       <c r="AA11" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>756.81818181818187</v>
       </c>
       <c r="AB11" s="4">
@@ -1477,22 +1477,22 @@
         <v>0.53343039534102354</v>
       </c>
       <c r="D12" s="3" t="e">
-        <f>Q12/I12</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="E12" s="3">
         <v>70.5</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29.5</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>544.77272727272714</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>227.95454545454541</v>
       </c>
       <c r="I12" s="3">
@@ -1505,7 +1505,7 @@
         <v>18132919837914.695</v>
       </c>
       <c r="L12" s="5">
-        <f>K12-I12/X12</f>
+        <f t="shared" si="3"/>
         <v>18132919837795.641</v>
       </c>
       <c r="M12" s="1">
@@ -1518,11 +1518,11 @@
         <v>24</v>
       </c>
       <c r="P12" s="3" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="Q12" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="R12" s="1">
@@ -1547,15 +1547,15 @@
         <v>7.5000000064999996</v>
       </c>
       <c r="Y12" s="2">
-        <f>E12/100*(J12/I12)</f>
+        <f t="shared" si="9"/>
         <v>8.7246612162616172E-2</v>
       </c>
       <c r="Z12" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.2476265539254112</v>
       </c>
       <c r="AA12" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>772.72727272727263</v>
       </c>
       <c r="AB12" s="4">
@@ -1574,22 +1574,22 @@
         <v>0.52217873450750152</v>
       </c>
       <c r="D13" s="3">
-        <f>Q13/I13</f>
+        <f t="shared" si="1"/>
         <v>0.14197030410337649</v>
       </c>
       <c r="E13" s="3">
         <v>71.5</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28.5</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>570.60714285714278</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>227.44480519480516</v>
       </c>
       <c r="I13" s="3">
@@ -1602,7 +1602,7 @@
         <v>18907001439556.965</v>
       </c>
       <c r="L13" s="5">
-        <f>K13-I13/X13</f>
+        <f t="shared" si="3"/>
         <v>18907001439433.109</v>
       </c>
       <c r="M13" s="1">
@@ -1615,11 +1615,11 @@
         <v>28.3</v>
       </c>
       <c r="P13" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.80857142857142861</v>
       </c>
       <c r="Q13" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>130.58428571428573</v>
       </c>
       <c r="R13" s="1">
@@ -1644,15 +1644,15 @@
         <v>7.4263379687119402</v>
       </c>
       <c r="Y13" s="2">
-        <f>E13/100*(J13/I13)</f>
+        <f t="shared" si="9"/>
         <v>9.5535442487497277E-2</v>
       </c>
       <c r="Z13" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.471245814307458</v>
       </c>
       <c r="AA13" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>798.05194805194799</v>
       </c>
       <c r="AB13" s="4">
@@ -1671,22 +1671,22 @@
         <v>0.50277225651218749</v>
       </c>
       <c r="D14" s="3">
-        <f>Q14/I14</f>
+        <f t="shared" si="1"/>
         <v>0.15425692712907818</v>
       </c>
       <c r="E14" s="3">
         <v>69.2</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30.799999999999997</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>573.25443786982271</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>255.14792899408289</v>
       </c>
       <c r="I14" s="3">
@@ -1699,7 +1699,7 @@
         <v>19969099209988.664</v>
       </c>
       <c r="L14" s="5">
-        <f>K14-I14/X14</f>
+        <f t="shared" si="3"/>
         <v>19969099209851.109</v>
       </c>
       <c r="M14" s="1">
@@ -1712,11 +1712,11 @@
         <v>34.700000000000003</v>
       </c>
       <c r="P14" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.83213429256594729</v>
       </c>
       <c r="Q14" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>147.45419664268584</v>
       </c>
       <c r="R14" s="1">
@@ -1741,15 +1741,15 @@
         <v>6.9492916656666699</v>
       </c>
       <c r="Y14" s="2">
-        <f>E14/100*(J14/I14)</f>
+        <f t="shared" si="9"/>
         <v>0.10134951354744219</v>
       </c>
       <c r="Z14" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.7128067789517729</v>
       </c>
       <c r="AA14" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>828.40236686390551</v>
       </c>
       <c r="AB14" s="4">
@@ -1768,22 +1768,22 @@
         <v>0.51949748743718593</v>
       </c>
       <c r="D15" s="3">
-        <f>Q15/I15</f>
+        <f t="shared" si="1"/>
         <v>0.15976724627320707</v>
       </c>
       <c r="E15" s="3">
         <v>68</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>591.63636363636374</v>
       </c>
       <c r="H15" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>278.41711229946526</v>
       </c>
       <c r="I15" s="3">
@@ -1796,7 +1796,7 @@
         <v>21250667274470.809</v>
       </c>
       <c r="L15" s="5">
-        <f>K15-I15/X15</f>
+        <f t="shared" si="3"/>
         <v>21250667274306.332</v>
       </c>
       <c r="M15" s="1">
@@ -1809,11 +1809,11 @@
         <v>40.700000000000003</v>
       </c>
       <c r="P15" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.85146443514644365</v>
       </c>
       <c r="Q15" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>158.96841004184103</v>
       </c>
       <c r="R15" s="1">
@@ -1838,15 +1838,15 @@
         <v>6.049499999</v>
       </c>
       <c r="Y15" s="2">
-        <f>E15/100*(J15/I15)</f>
+        <f t="shared" si="9"/>
         <v>0.11119195979899497</v>
       </c>
       <c r="Z15" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.0792896482412058</v>
       </c>
       <c r="AA15" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>870.05347593582894</v>
       </c>
       <c r="AB15" s="4">
@@ -1865,22 +1865,22 @@
         <v>0.51346681573330621</v>
       </c>
       <c r="D16" s="3">
-        <f>Q16/I16</f>
+        <f t="shared" si="1"/>
         <v>0.14819935585754634</v>
       </c>
       <c r="E16" s="3">
         <v>70.100000000000009</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29.899999999999991</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>611.72169811320771</v>
       </c>
       <c r="H16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>260.91981132075466</v>
       </c>
       <c r="I16" s="3">
@@ -1893,7 +1893,7 @@
         <v>21644518137331.043</v>
       </c>
       <c r="L16" s="5">
-        <f>K16-I16/X16</f>
+        <f t="shared" si="3"/>
         <v>21644518137169.613</v>
       </c>
       <c r="M16" s="1">
@@ -1906,11 +1906,11 @@
         <v>43.5</v>
       </c>
       <c r="P16" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.8413926499032881</v>
       </c>
       <c r="Q16" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>145.81334622823985</v>
       </c>
       <c r="R16" s="1">
@@ -1935,15 +1935,15 @@
         <v>6.0948999989999999</v>
       </c>
       <c r="Y16" s="2">
-        <f>E16/100*(J16/I16)</f>
+        <f t="shared" si="9"/>
         <v>0.13180709421689196</v>
       </c>
       <c r="Z16" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.7943103973981094</v>
       </c>
       <c r="AA16" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>872.64150943396237</v>
       </c>
       <c r="AB16" s="4">
@@ -1962,22 +1962,22 @@
         <v>0.53749355337802995</v>
       </c>
       <c r="D17" s="3">
-        <f>Q17/I17</f>
+        <f t="shared" si="1"/>
         <v>0.13266715755395037</v>
       </c>
       <c r="E17" s="3">
         <v>70.900000000000006</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29.099999999999994</v>
       </c>
       <c r="G17" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>606.19499999999994</v>
       </c>
       <c r="H17" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>248.80499999999989</v>
       </c>
       <c r="I17" s="3">
@@ -1990,7 +1990,7 @@
         <v>21789950800692.965</v>
       </c>
       <c r="L17" s="5">
-        <f>K17-I17/X17</f>
+        <f t="shared" si="3"/>
         <v>21789950800524.242</v>
       </c>
       <c r="M17" s="1">
@@ -2003,11 +2003,11 @@
         <v>42.6</v>
       </c>
       <c r="P17" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.82080924855491311</v>
       </c>
       <c r="Q17" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>128.62080924855488</v>
       </c>
       <c r="R17" s="1">
@@ -2032,15 +2032,15 @@
         <v>5.746149999</v>
       </c>
       <c r="Y17" s="2">
-        <f>E17/100*(J17/I17)</f>
+        <f t="shared" si="9"/>
         <v>0.15006374419804025</v>
       </c>
       <c r="Z17" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.601529860752966</v>
       </c>
       <c r="AA17" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>854.99999999999989</v>
       </c>
       <c r="AB17" s="4">
@@ -2059,22 +2059,22 @@
         <v>0.54605647517039924</v>
       </c>
       <c r="D18" s="3">
-        <f>Q18/I18</f>
+        <f t="shared" si="1"/>
         <v>0.14960245159825805</v>
       </c>
       <c r="E18" s="3">
         <v>70</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>632.93893129770993</v>
       </c>
       <c r="H18" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>271.25954198473283</v>
       </c>
       <c r="I18" s="3">
@@ -2087,7 +2087,7 @@
         <v>22950162752510.637</v>
       </c>
       <c r="L18" s="5">
-        <f>K18-I18/X18</f>
+        <f t="shared" si="3"/>
         <v>22950162752340.746</v>
       </c>
       <c r="M18" s="1">
@@ -2100,11 +2100,11 @@
         <v>54.8</v>
       </c>
       <c r="P18" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.84049079754601219</v>
       </c>
       <c r="Q18" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>153.64171779141103</v>
       </c>
       <c r="R18" s="1">
@@ -2129,15 +2129,15 @@
         <v>6.0450249989999998</v>
       </c>
       <c r="Y18" s="2">
-        <f>E18/100*(J18/I18)</f>
+        <f t="shared" si="9"/>
         <v>0.16147030185004868</v>
       </c>
       <c r="Z18" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.2305219084712755</v>
       </c>
       <c r="AA18" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>904.19847328244282</v>
       </c>
       <c r="AB18" s="4">
@@ -2156,22 +2156,22 @@
         <v>0.54674058497419231</v>
       </c>
       <c r="D19" s="3">
-        <f>Q19/I19</f>
+        <f t="shared" si="1"/>
         <v>0.14415121391703306</v>
       </c>
       <c r="E19" s="3">
         <v>70.2</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29.799999999999997</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>639.90000000000009</v>
       </c>
       <c r="H19" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>271.63846153846151</v>
       </c>
       <c r="I19" s="3">
@@ -2184,7 +2184,7 @@
         <v>23888075049016.668</v>
       </c>
       <c r="L19" s="5">
-        <f>K19-I19/X19</f>
+        <f t="shared" si="3"/>
         <v>23888075048842.395</v>
       </c>
       <c r="M19" s="1">
@@ -2197,11 +2197,11 @@
         <v>58.1</v>
       </c>
       <c r="P19" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.83000000000000007</v>
       </c>
       <c r="Q19" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>150.81100000000001</v>
       </c>
       <c r="R19" s="1">
@@ -2226,15 +2226,15 @@
         <v>6.0031916656666704</v>
       </c>
       <c r="Y19" s="2">
-        <f>E19/100*(J19/I19)</f>
+        <f t="shared" si="9"/>
         <v>0.17492965016249282</v>
       </c>
       <c r="Z19" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.0029879946472944</v>
       </c>
       <c r="AA19" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>911.53846153846155</v>
       </c>
       <c r="AB19" s="4">
@@ -2253,22 +2253,22 @@
         <v>0.54399251986909791</v>
       </c>
       <c r="D20" s="3">
-        <f>Q20/I20</f>
+        <f t="shared" si="1"/>
         <v>0.14378317873826496</v>
       </c>
       <c r="E20" s="3">
         <v>70.3</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29.700000000000003</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>649.65337620578771</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>274.4623794212219</v>
       </c>
       <c r="I20" s="3">
@@ -2281,7 +2281,7 @@
         <v>24875201431284.375</v>
       </c>
       <c r="L20" s="5">
-        <f>K20-I20/X20</f>
+        <f t="shared" si="3"/>
         <v>24875201431090.438</v>
       </c>
       <c r="M20" s="1">
@@ -2294,11 +2294,11 @@
         <v>63.5</v>
       </c>
       <c r="P20" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.82898172323759778</v>
       </c>
       <c r="Q20" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>153.77610966057438</v>
       </c>
       <c r="R20" s="1">
@@ -2323,15 +2323,15 @@
         <v>5.5146249989999996</v>
       </c>
       <c r="Y20" s="2">
-        <f>E20/100*(J20/I20)</f>
+        <f t="shared" si="9"/>
         <v>0.18891276297335202</v>
       </c>
       <c r="Z20" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.8751869284712486</v>
       </c>
       <c r="AA20" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>924.11575562700955</v>
       </c>
       <c r="AB20" s="4">
@@ -2350,22 +2350,22 @@
         <v>0.52912053290125138</v>
       </c>
       <c r="D21" s="3">
-        <f>Q21/I21</f>
+        <f t="shared" si="1"/>
         <v>0.13669298496823221</v>
       </c>
       <c r="E21" s="3">
         <v>70.900000000000006</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29.099999999999994</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>673.86936936936945</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>276.58108108108104</v>
       </c>
       <c r="I21" s="3">
@@ -2378,7 +2378,7 @@
         <v>25913470306521.648</v>
       </c>
       <c r="L21" s="5">
-        <f>K21-I21/X21</f>
+        <f t="shared" si="3"/>
         <v>25913470306310.488</v>
       </c>
       <c r="M21" s="1">
@@ -2391,11 +2391,11 @@
         <v>67.3</v>
       </c>
       <c r="P21" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.81378476420798063</v>
       </c>
       <c r="Q21" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>151.85223700120918</v>
       </c>
       <c r="R21" s="1">
@@ -2420,15 +2420,15 @@
         <v>5.2609583323333302</v>
       </c>
       <c r="Y21" s="2">
-        <f>E21/100*(J21/I21)</f>
+        <f t="shared" si="9"/>
         <v>0.20199702943559278</v>
       </c>
       <c r="Z21" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6.7265010802052387</v>
       </c>
       <c r="AA21" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>950.45045045045049</v>
       </c>
       <c r="AB21" s="4">
@@ -2447,22 +2447,22 @@
         <v>0.51985526910900048</v>
       </c>
       <c r="D22" s="3">
-        <f>Q22/I22</f>
+        <f t="shared" si="1"/>
         <v>0.12449548267531521</v>
       </c>
       <c r="E22" s="3">
         <v>71.5</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28.5</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>676.78787878787887</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>269.76859504132233</v>
       </c>
       <c r="I22" s="3">
@@ -2475,7 +2475,7 @@
         <v>26405447512716.551</v>
       </c>
       <c r="L22" s="5">
-        <f>K22-I22/X22</f>
+        <f t="shared" si="3"/>
         <v>26405447512520.398</v>
       </c>
       <c r="M22" s="1">
@@ -2488,11 +2488,11 @@
         <v>66.7</v>
       </c>
       <c r="P22" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.81341463414634152</v>
       </c>
       <c r="Q22" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>137.62975609756097</v>
       </c>
       <c r="R22" s="1">
@@ -2517,15 +2517,15 @@
         <v>5.6359416656666701</v>
       </c>
       <c r="Y22" s="2">
-        <f>E22/100*(J22/I22)</f>
+        <f t="shared" si="9"/>
         <v>0.22222885572139303</v>
       </c>
       <c r="Z22" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8.0669074626865669</v>
       </c>
       <c r="AA22" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>946.55647382920131</v>
       </c>
       <c r="AB22" s="4">
@@ -2544,22 +2544,22 @@
         <v>0.516801748474638</v>
       </c>
       <c r="D23" s="3">
-        <f>Q23/I23</f>
+        <f t="shared" si="1"/>
         <v>0.10227811146789778</v>
       </c>
       <c r="E23" s="3">
         <v>70.3</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29.700000000000003</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>664.0807980049874</v>
       </c>
       <c r="H23" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>280.55760598503741</v>
       </c>
       <c r="I23" s="3">
@@ -2572,7 +2572,7 @@
         <v>26936752594348.961</v>
       </c>
       <c r="L23" s="5">
-        <f>K23-I23/X23</f>
+        <f t="shared" si="3"/>
         <v>26936752594194.805</v>
       </c>
       <c r="M23" s="1">
@@ -2585,11 +2585,11 @@
         <v>60.5</v>
       </c>
       <c r="P23" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.79710144927536231</v>
       </c>
       <c r="Q23" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>112.31159420289855</v>
       </c>
       <c r="R23" s="1">
@@ -2614,15 +2614,15 @@
         <v>7.1233666656666701</v>
       </c>
       <c r="Y23" s="2">
-        <f>E23/100*(J23/I23)</f>
+        <f t="shared" si="9"/>
         <v>0.24250651124669886</v>
       </c>
       <c r="Z23" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.7245111009926255</v>
       </c>
       <c r="AA23" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>944.63840399002481</v>
       </c>
       <c r="AB23" s="4">
@@ -2641,22 +2641,22 @@
         <v>0.50544528368171437</v>
       </c>
       <c r="D24" s="3">
-        <f>Q24/I24</f>
+        <f t="shared" si="1"/>
         <v>0.11064445615473194</v>
       </c>
       <c r="E24" s="3">
         <v>68.8</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31.200000000000003</v>
       </c>
       <c r="G24" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>680.21719457013558</v>
       </c>
       <c r="H24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>308.47058823529414</v>
       </c>
       <c r="I24" s="3">
@@ -2669,7 +2669,7 @@
         <v>27017667672121.348</v>
       </c>
       <c r="L24" s="5">
-        <f>K24-I24/X24</f>
+        <f t="shared" si="3"/>
         <v>27017667671984.699</v>
       </c>
       <c r="M24" s="1">
@@ -2682,11 +2682,11 @@
         <v>74.3</v>
       </c>
       <c r="P24" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.82555555555555549</v>
       </c>
       <c r="Q24" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>125.97977777777777</v>
       </c>
       <c r="R24" s="1">
@@ -2711,15 +2711,15 @@
         <v>8.3324416661666696</v>
       </c>
       <c r="Y24" s="2">
-        <f>E24/100*(J24/I24)</f>
+        <f t="shared" si="9"/>
         <v>0.26405761461443877</v>
       </c>
       <c r="Z24" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>11.671346565958194</v>
       </c>
       <c r="AA24" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>988.68778280542972</v>
       </c>
       <c r="AB24" s="4">
@@ -2738,22 +2738,22 @@
         <v>0.50209742316582484</v>
       </c>
       <c r="D25" s="3">
-        <f>Q25/I25</f>
+        <f t="shared" si="1"/>
         <v>0.11588508957651603</v>
       </c>
       <c r="E25" s="3">
         <v>68.100000000000009</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31.899999999999991</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>689.60210526315791</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>323.02947368421042</v>
       </c>
       <c r="I25" s="3">
@@ -2766,7 +2766,7 @@
         <v>27720880247609.52</v>
       </c>
       <c r="L25" s="5">
-        <f>K25-I25/X25</f>
+        <f t="shared" si="3"/>
         <v>27720880247481.789</v>
       </c>
       <c r="M25" s="1">
@@ -2779,11 +2779,11 @@
         <v>85.4</v>
       </c>
       <c r="P25" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.84975124378109457</v>
       </c>
       <c r="Q25" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>135.36537313432837</v>
       </c>
       <c r="R25" s="1">
@@ -2808,15 +2808,15 @@
         <v>9.1449916657500001</v>
       </c>
       <c r="Y25" s="2">
-        <f>E25/100*(J25/I25)</f>
+        <f t="shared" si="9"/>
         <v>0.2804220529064293</v>
       </c>
       <c r="Z25" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>13.320047513055391</v>
       </c>
       <c r="AA25" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1012.6315789473684</v>
       </c>
       <c r="AB25" s="4">
@@ -2835,22 +2835,22 @@
         <v>0.49893162393162399</v>
       </c>
       <c r="D26" s="3">
-        <f>Q26/I26</f>
+        <f t="shared" si="1"/>
         <v>0.12436964964720716</v>
       </c>
       <c r="E26" s="3">
         <v>66.3</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33.700000000000003</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>698.58846918489064</v>
       </c>
       <c r="H26" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>355.08946322067601</v>
       </c>
       <c r="I26" s="3">
@@ -2863,7 +2863,7 @@
         <v>29026887759048.16</v>
       </c>
       <c r="L26" s="5">
-        <f>K26-I26/X26</f>
+        <f t="shared" si="3"/>
         <v>29026887758930.668</v>
       </c>
       <c r="M26" s="1">
@@ -2876,11 +2876,11 @@
         <v>100.2</v>
       </c>
       <c r="P26" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.86082474226804118</v>
       </c>
       <c r="Q26" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>151.33298969072166</v>
       </c>
       <c r="R26" s="1">
@@ -2905,15 +2905,15 @@
         <v>10.356591666250001</v>
       </c>
       <c r="Y26" s="2">
-        <f>E26/100*(J26/I26)</f>
+        <f t="shared" si="9"/>
         <v>0.28878205128205126</v>
       </c>
       <c r="Z26" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>14.525737179487177</v>
       </c>
       <c r="AA26" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1053.6779324055667</v>
       </c>
       <c r="AB26" s="4">
@@ -2932,22 +2932,22 @@
         <v>0.50130383247728183</v>
       </c>
       <c r="D27" s="3">
-        <f>Q27/I27</f>
+        <f t="shared" si="1"/>
         <v>0.13594449237616818</v>
       </c>
       <c r="E27" s="3">
         <v>66.2</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33.799999999999997</v>
       </c>
       <c r="G27" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>720.76038095238107</v>
       </c>
       <c r="H27" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>368.0015238095238</v>
       </c>
       <c r="I27" s="3">
@@ -2960,7 +2960,7 @@
         <v>30106081598977.883</v>
       </c>
       <c r="L27" s="5">
-        <f>K27-I27/X27</f>
+        <f t="shared" si="3"/>
         <v>30106081598858.457</v>
       </c>
       <c r="M27" s="1">
@@ -2973,11 +2973,11 @@
         <v>117.9</v>
       </c>
       <c r="P27" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.85932944606414008</v>
       </c>
       <c r="Q27" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>172.03775510204085</v>
       </c>
       <c r="R27" s="1">
@@ -3002,15 +3002,15 @@
         <v>10.5963916664167</v>
       </c>
       <c r="Y27" s="2">
-        <f>E27/100*(J27/I27)</f>
+        <f t="shared" si="9"/>
         <v>0.29901161596207032</v>
       </c>
       <c r="Z27" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>15.698109838008692</v>
       </c>
       <c r="AA27" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1088.7619047619048</v>
       </c>
       <c r="AB27" s="4">
@@ -3029,22 +3029,22 @@
         <v>0.51190117505272681</v>
       </c>
       <c r="D28" s="3">
-        <f>Q28/I28</f>
+        <f t="shared" si="1"/>
         <v>0.15790280118743039</v>
       </c>
       <c r="E28" s="3">
         <v>67.2</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32.799999999999997</v>
       </c>
       <c r="G28" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>755.46815642458114</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>368.74040968342644</v>
       </c>
       <c r="I28" s="3">
@@ -3057,7 +3057,7 @@
         <v>31122654330255.297</v>
       </c>
       <c r="L28" s="5">
-        <f>K28-I28/X28</f>
+        <f t="shared" si="3"/>
         <v>31122654330091.215</v>
       </c>
       <c r="M28" s="1">
@@ -3070,11 +3070,11 @@
         <v>142.5</v>
       </c>
       <c r="P28" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.88564325668116839</v>
       </c>
       <c r="Q28" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>209.63175885643255</v>
       </c>
       <c r="R28" s="1">
@@ -3099,15 +3099,15 @@
         <v>8.0909916665833403</v>
       </c>
       <c r="Y28" s="2">
-        <f>E28/100*(J28/I28)</f>
+        <f t="shared" si="9"/>
         <v>0.30557878879180483</v>
       </c>
       <c r="Z28" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>16.409580958119921</v>
       </c>
       <c r="AA28" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1124.2085661080075</v>
       </c>
       <c r="AB28" s="4">
@@ -3126,22 +3126,22 @@
         <v>0.50082644628099171</v>
       </c>
       <c r="D29" s="3">
-        <f>Q29/I29</f>
+        <f t="shared" si="1"/>
         <v>0.16084097917624501</v>
       </c>
       <c r="E29" s="3">
         <v>69</v>
       </c>
       <c r="F29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="G29" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>780.11743772241994</v>
       </c>
       <c r="H29" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>350.4875444839858</v>
       </c>
       <c r="I29" s="3">
@@ -3154,7 +3154,7 @@
         <v>32287869900775.047</v>
       </c>
       <c r="L29" s="5">
-        <f>K29-I29/X29</f>
+        <f t="shared" si="3"/>
         <v>32287869900580.465</v>
       </c>
       <c r="M29" s="1">
@@ -3167,11 +3167,11 @@
         <v>146.9</v>
       </c>
       <c r="P29" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.87701492537313441</v>
       </c>
       <c r="Q29" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>214.07934328358212</v>
       </c>
       <c r="R29" s="1">
@@ -3196,15 +3196,15 @@
         <v>6.8403166666666699</v>
       </c>
       <c r="Y29" s="2">
-        <f>E29/100*(J29/I29)</f>
+        <f t="shared" si="9"/>
         <v>0.32939594290007518</v>
       </c>
       <c r="Z29" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>18.512051990984226</v>
       </c>
       <c r="AA29" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1130.6049822064058</v>
       </c>
       <c r="AB29" s="4">
@@ -3223,22 +3223,22 @@
         <v>0.49173429516080563</v>
       </c>
       <c r="D30" s="3">
-        <f>Q30/I30</f>
+        <f t="shared" si="1"/>
         <v>0.1482860772914559</v>
       </c>
       <c r="E30" s="3">
         <v>69.3</v>
       </c>
       <c r="F30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30.700000000000003</v>
       </c>
       <c r="G30" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>789.7114726027396</v>
       </c>
       <c r="H30" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>349.84332191780823</v>
       </c>
       <c r="I30" s="3">
@@ -3251,7 +3251,7 @@
         <v>33781478943684.832</v>
       </c>
       <c r="L30" s="5">
-        <f>K30-I30/X30</f>
+        <f t="shared" si="3"/>
         <v>33781478943487.137</v>
       </c>
       <c r="M30" s="1">
@@ -3264,11 +3264,11 @@
         <v>138.9</v>
       </c>
       <c r="P30" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.85687847008019746</v>
       </c>
       <c r="Q30" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>197.33911165946949</v>
       </c>
       <c r="R30" s="1">
@@ -3293,15 +3293,15 @@
         <v>6.7315250000000004</v>
       </c>
       <c r="Y30" s="2">
-        <f>E30/100*(J30/I30)</f>
+        <f t="shared" si="9"/>
         <v>0.34655207394048693</v>
       </c>
       <c r="Z30" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>20.238641118124438</v>
       </c>
       <c r="AA30" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1139.5547945205478</v>
       </c>
       <c r="AB30" s="4">
@@ -3320,22 +3320,22 @@
         <v>0.49014484097357019</v>
       </c>
       <c r="D31" s="3">
-        <f>Q31/I31</f>
+        <f t="shared" si="1"/>
         <v>0.15211980567503974</v>
       </c>
       <c r="E31" s="3">
         <v>67.400000000000006</v>
       </c>
       <c r="F31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32.599999999999994</v>
       </c>
       <c r="G31" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>779.82019543973956</v>
       </c>
       <c r="H31" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>377.18306188925084</v>
       </c>
       <c r="I31" s="3">
@@ -3348,7 +3348,7 @@
         <v>35035086233597.582</v>
       </c>
       <c r="L31" s="5">
-        <f>K31-I31/X31</f>
+        <f t="shared" si="3"/>
         <v>35035086233414.359</v>
       </c>
       <c r="M31" s="1">
@@ -3361,11 +3361,11 @@
         <v>148</v>
       </c>
       <c r="P31" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.86701816051552438</v>
       </c>
       <c r="Q31" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>203.74926772114824</v>
       </c>
       <c r="R31" s="1">
@@ -3390,15 +3390,15 @@
         <v>7.3101750000000001</v>
       </c>
       <c r="Y31" s="2">
-        <f>E31/100*(J31/I31)</f>
+        <f t="shared" si="9"/>
         <v>0.3574806629834254</v>
       </c>
       <c r="Z31" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>21.949312707182319</v>
       </c>
       <c r="AA31" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1157.0032573289905</v>
       </c>
       <c r="AB31" s="4">
@@ -3417,22 +3417,22 @@
         <v>0.48693988668972132</v>
       </c>
       <c r="D32" s="3">
-        <f>Q32/I32</f>
+        <f t="shared" si="1"/>
         <v>0.14982493928753568</v>
       </c>
       <c r="E32" s="3">
         <v>66.5</v>
       </c>
       <c r="F32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33.5</v>
       </c>
       <c r="G32" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>787.63910969793324</v>
       </c>
       <c r="H32" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>396.7806041335453</v>
       </c>
       <c r="I32" s="3">
@@ -3445,7 +3445,7 @@
         <v>36018965412718.43</v>
       </c>
       <c r="L32" s="5">
-        <f>K32-I32/X32</f>
+        <f t="shared" si="3"/>
         <v>36018965412498.812</v>
       </c>
       <c r="M32" s="1">
@@ -3458,11 +3458,11 @@
         <v>151.69999999999999</v>
       </c>
       <c r="P32" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.8683457355466514</v>
       </c>
       <c r="Q32" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>203.62707498568975</v>
       </c>
       <c r="R32" s="1">
@@ -3487,15 +3487,15 @@
         <v>6.1885583333333303</v>
       </c>
       <c r="Y32" s="2">
-        <f>E32/100*(J32/I32)</f>
+        <f t="shared" si="9"/>
         <v>0.36452431756309328</v>
       </c>
       <c r="Z32" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>22.928579574718565</v>
       </c>
       <c r="AA32" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1184.4197138314785</v>
       </c>
       <c r="AB32" s="4">
@@ -3514,22 +3514,22 @@
         <v>0.4879907118496481</v>
       </c>
       <c r="D33" s="3">
-        <f>Q33/I33</f>
+        <f t="shared" si="1"/>
         <v>0.14510153772959294</v>
       </c>
       <c r="E33" s="3">
         <v>66</v>
       </c>
       <c r="F33" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="G33" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>792.61300309597527</v>
       </c>
       <c r="H33" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>408.31578947368422</v>
       </c>
       <c r="I33" s="3">
@@ -3542,7 +3542,7 @@
         <v>36514450772121.398</v>
       </c>
       <c r="L33" s="5">
-        <f>K33-I33/X33</f>
+        <f t="shared" si="3"/>
         <v>36514450771905.953</v>
       </c>
       <c r="M33" s="1">
@@ -3555,11 +3555,11 @@
         <v>152.19999999999999</v>
       </c>
       <c r="P33" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.87320711417096952</v>
       </c>
       <c r="Q33" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>199.96442914515202</v>
       </c>
       <c r="R33" s="1">
@@ -3584,15 +3584,15 @@
         <v>6.3964583333333298</v>
       </c>
       <c r="Y33" s="2">
-        <f>E33/100*(J33/I33)</f>
+        <f t="shared" si="9"/>
         <v>0.37154633190624786</v>
       </c>
       <c r="Z33" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>24.001893041143614</v>
       </c>
       <c r="AA33" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1200.9287925696594</v>
       </c>
       <c r="AB33" s="4">
@@ -3607,26 +3607,26 @@
         <v>689.80000000000018</v>
       </c>
       <c r="C34" s="3">
-        <f t="shared" ref="C34:C64" si="8">B34/I34</f>
+        <f t="shared" ref="C34:C64" si="11">B34/I34</f>
         <v>0.49096085409252682</v>
       </c>
       <c r="D34" s="3">
-        <f>Q34/I34</f>
+        <f t="shared" ref="D34:D64" si="12">Q34/I34</f>
         <v>0.13741548300582804</v>
       </c>
       <c r="E34" s="3">
         <v>65.100000000000009</v>
       </c>
       <c r="F34" s="3">
-        <f t="shared" ref="F34:F64" si="9">100-E34</f>
+        <f t="shared" ref="F34:F64" si="13">100-E34</f>
         <v>34.899999999999991</v>
       </c>
       <c r="G34" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>802.99908675799122</v>
       </c>
       <c r="H34" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>430.48645357686451</v>
       </c>
       <c r="I34" s="3">
@@ -3639,7 +3639,7 @@
         <v>37262121337902.93</v>
       </c>
       <c r="L34" s="5">
-        <f>K34-I34/X34</f>
+        <f t="shared" ref="L34:L65" si="14">K34-I34/X34</f>
         <v>37262121337670.164</v>
       </c>
       <c r="M34" s="1">
@@ -3652,11 +3652,11 @@
         <v>146.19999999999999</v>
       </c>
       <c r="P34" s="3">
-        <f t="shared" ref="P34:P64" si="10">O34/N34</f>
+        <f t="shared" ref="P34:P64" si="15">O34/N34</f>
         <v>0.84753623188405791</v>
       </c>
       <c r="Q34" s="3">
-        <f t="shared" ref="Q34:Q64" si="11">P34*M34</f>
+        <f t="shared" ref="Q34:Q64" si="16">P34*M34</f>
         <v>193.0687536231884</v>
       </c>
       <c r="R34" s="1">
@@ -3681,15 +3681,15 @@
         <v>6.0361333333333302</v>
       </c>
       <c r="Y34" s="2">
-        <f>E34/100*(J34/I34)</f>
+        <f t="shared" si="9"/>
         <v>0.37549494661921717</v>
       </c>
       <c r="Z34" s="3">
-        <f t="shared" ref="Z34:Z64" si="12">Y34*S34</f>
+        <f t="shared" si="6"/>
         <v>24.67001799288257</v>
       </c>
       <c r="AA34" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1233.4855403348556</v>
       </c>
       <c r="AB34" s="4">
@@ -3704,26 +3704,26 @@
         <v>683.80000000000018</v>
       </c>
       <c r="C35" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.48662112154853415</v>
       </c>
       <c r="D35" s="3">
-        <f>Q35/I35</f>
+        <f t="shared" si="12"/>
         <v>0.13374711290426342</v>
       </c>
       <c r="E35" s="3">
         <v>65.400000000000006</v>
       </c>
       <c r="F35" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>34.599999999999994</v>
       </c>
       <c r="G35" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>802.8072617246595</v>
       </c>
       <c r="H35" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>424.72677760968213</v>
       </c>
       <c r="I35" s="3">
@@ -3736,7 +3736,7 @@
         <v>37949171730790.43</v>
       </c>
       <c r="L35" s="5">
-        <f>K35-I35/X35</f>
+        <f t="shared" si="14"/>
         <v>37949171730573.711</v>
       </c>
       <c r="M35" s="1">
@@ -3749,11 +3749,11 @@
         <v>142.1</v>
       </c>
       <c r="P35" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.84734645199761482</v>
       </c>
       <c r="Q35" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>187.94144305307097</v>
       </c>
       <c r="R35" s="1">
@@ -3778,15 +3778,15 @@
         <v>6.4839391666666701</v>
       </c>
       <c r="Y35" s="2">
-        <f>E35/100*(J35/I35)</f>
+        <f t="shared" si="9"/>
         <v>0.37763706233988048</v>
       </c>
       <c r="Z35" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>24.961809820666105</v>
       </c>
       <c r="AA35" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1227.5340393343417</v>
       </c>
       <c r="AB35" s="4">
@@ -3801,26 +3801,26 @@
         <v>729.30000000000018</v>
       </c>
       <c r="C36" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.4927369772312683</v>
       </c>
       <c r="D36" s="3">
-        <f>Q36/I36</f>
+        <f t="shared" si="12"/>
         <v>0.13607924538146673</v>
       </c>
       <c r="E36" s="3">
         <v>63.1</v>
       </c>
       <c r="F36" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>36.9</v>
       </c>
       <c r="G36" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>810.80208643815195</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>474.14575260804764</v>
       </c>
       <c r="I36" s="3">
@@ -3833,7 +3833,7 @@
         <v>39211384629028.148</v>
       </c>
       <c r="L36" s="5">
-        <f>K36-I36/X36</f>
+        <f t="shared" si="14"/>
         <v>39211384628795.445</v>
       </c>
       <c r="M36" s="1">
@@ -3846,11 +3846,11 @@
         <v>154.5</v>
       </c>
       <c r="P36" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.84983498349834974</v>
       </c>
       <c r="Q36" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>201.4108910891089</v>
       </c>
       <c r="R36" s="1">
@@ -3875,15 +3875,15 @@
         <v>6.3605516666666704</v>
       </c>
       <c r="Y36" s="2">
-        <f>E36/100*(J36/I36)</f>
+        <f t="shared" si="9"/>
         <v>0.3675752989662861</v>
       </c>
       <c r="Z36" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>24.6643025606378</v>
       </c>
       <c r="AA36" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1284.9478390461995</v>
       </c>
       <c r="AB36" s="4">
@@ -3898,26 +3898,26 @@
         <v>741.6</v>
       </c>
       <c r="C37" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.48632697226047611</v>
       </c>
       <c r="D37" s="3">
-        <f>Q37/I37</f>
+        <f t="shared" si="12"/>
         <v>0.14642586035326866</v>
       </c>
       <c r="E37" s="3">
         <v>63.1</v>
       </c>
       <c r="F37" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>36.9</v>
       </c>
       <c r="G37" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>833.75514705882347</v>
       </c>
       <c r="H37" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>487.56838235294117</v>
       </c>
       <c r="I37" s="3">
@@ -3930,7 +3930,7 @@
         <v>40418697808330.289</v>
       </c>
       <c r="L37" s="5">
-        <f>K37-I37/X37</f>
+        <f t="shared" si="14"/>
         <v>40418697808058.102</v>
       </c>
       <c r="M37" s="1">
@@ -3943,11 +3943,11 @@
         <v>172</v>
       </c>
       <c r="P37" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.85190688459633479</v>
       </c>
       <c r="Q37" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>223.28479445269937</v>
       </c>
       <c r="R37" s="1">
@@ -3972,15 +3972,15 @@
         <v>5.6023666666666703</v>
       </c>
       <c r="Y37" s="2">
-        <f>E37/100*(J37/I37)</f>
+        <f t="shared" si="9"/>
         <v>0.371797167027346</v>
       </c>
       <c r="Z37" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>25.282207357859527</v>
       </c>
       <c r="AA37" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1321.3235294117646</v>
       </c>
       <c r="AB37" s="4">
@@ -3995,26 +3995,26 @@
         <v>759.80000000000018</v>
       </c>
       <c r="C38" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.48419576854448138</v>
       </c>
       <c r="D38" s="3">
-        <f>Q38/I38</f>
+        <f t="shared" si="12"/>
         <v>0.14850929621658557</v>
       </c>
       <c r="E38" s="3">
         <v>63.4</v>
       </c>
       <c r="F38" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>36.6</v>
       </c>
       <c r="G38" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>859.14776334776343</v>
       </c>
       <c r="H38" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>495.97489177489183</v>
       </c>
       <c r="I38" s="3">
@@ -4027,7 +4027,7 @@
         <v>41864956153669.422</v>
       </c>
       <c r="L38" s="5">
-        <f>K38-I38/X38</f>
+        <f t="shared" si="14"/>
         <v>41864956153398.805</v>
       </c>
       <c r="M38" s="1">
@@ -4040,11 +4040,11 @@
         <v>180.1</v>
       </c>
       <c r="P38" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.8443506797937177</v>
       </c>
       <c r="Q38" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>233.04078762306608</v>
       </c>
       <c r="R38" s="1">
@@ -4069,15 +4069,15 @@
         <v>5.79867166666667</v>
       </c>
       <c r="Y38" s="2">
-        <f>E38/100*(J38/I38)</f>
+        <f t="shared" si="9"/>
         <v>0.37942225337751723</v>
       </c>
       <c r="Z38" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>26.293962159061941</v>
       </c>
       <c r="AA38" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1355.1226551226553</v>
       </c>
       <c r="AB38" s="4">
@@ -4092,26 +4092,26 @@
         <v>782.2</v>
       </c>
       <c r="C39" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.48275010800469054</v>
       </c>
       <c r="D39" s="3">
-        <f>Q39/I39</f>
+        <f t="shared" si="12"/>
         <v>0.16130476598276713</v>
       </c>
       <c r="E39" s="3">
         <v>63.3</v>
       </c>
       <c r="F39" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>36.700000000000003</v>
       </c>
       <c r="G39" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>880.91753889674681</v>
       </c>
       <c r="H39" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>510.73734087694487</v>
       </c>
       <c r="I39" s="3">
@@ -4124,7 +4124,7 @@
         <v>43506495648007.766</v>
       </c>
       <c r="L39" s="5">
-        <f>K39-I39/X39</f>
+        <f t="shared" si="14"/>
         <v>43506495647762.43</v>
       </c>
       <c r="M39" s="1">
@@ -4137,11 +4137,11 @@
         <v>205</v>
       </c>
       <c r="P39" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.85917854149203687</v>
       </c>
       <c r="Q39" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>261.36211232187759</v>
       </c>
       <c r="R39" s="1">
@@ -4166,15 +4166,15 @@
         <v>6.6044591666666701</v>
       </c>
       <c r="Y39" s="2">
-        <f>E39/100*(J39/I39)</f>
+        <f t="shared" si="9"/>
         <v>0.38437863358637298</v>
       </c>
       <c r="Z39" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>27.175569394556572</v>
       </c>
       <c r="AA39" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1391.6548797736916</v>
       </c>
       <c r="AB39" s="4">
@@ -4189,26 +4189,26 @@
         <v>800.6</v>
       </c>
       <c r="C40" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.48336653987804146</v>
       </c>
       <c r="D40" s="3">
-        <f>Q40/I40</f>
+        <f t="shared" si="12"/>
         <v>0.17135681672607217</v>
       </c>
       <c r="E40" s="3">
         <v>65.2</v>
       </c>
       <c r="F40" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>34.799999999999997</v>
       </c>
       <c r="G40" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>917.53519553072613</v>
       </c>
       <c r="H40" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>489.72737430167587</v>
       </c>
       <c r="I40" s="3">
@@ -4221,7 +4221,7 @@
         <v>44749372724681.594</v>
       </c>
       <c r="L40" s="5">
-        <f>K40-I40/X40</f>
+        <f t="shared" si="14"/>
         <v>44749372724434.414</v>
       </c>
       <c r="M40" s="1">
@@ -4234,11 +4234,11 @@
         <v>223.8</v>
       </c>
       <c r="P40" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.87490226739640342</v>
       </c>
       <c r="Q40" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>283.81829554339333</v>
       </c>
       <c r="R40" s="1">
@@ -4263,15 +4263,15 @@
         <v>6.7008266666666696</v>
       </c>
       <c r="Y40" s="2">
-        <f>E40/100*(J40/I40)</f>
+        <f t="shared" si="9"/>
         <v>0.39664022218197187</v>
       </c>
       <c r="Z40" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>28.399439908229191</v>
       </c>
       <c r="AA40" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1407.2625698324021</v>
       </c>
       <c r="AB40" s="4">
@@ -4286,26 +4286,26 @@
         <v>799.6</v>
       </c>
       <c r="C41" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.46894610286786703</v>
       </c>
       <c r="D41" s="3">
-        <f>Q41/I41</f>
+        <f t="shared" si="12"/>
         <v>0.16488609778266733</v>
       </c>
       <c r="E41" s="3">
         <v>65.2</v>
       </c>
       <c r="F41" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>34.799999999999997</v>
       </c>
       <c r="G41" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>945.57912087912086</v>
       </c>
       <c r="H41" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>504.69560439560433</v>
       </c>
       <c r="I41" s="3">
@@ -4318,7 +4318,7 @@
         <v>46340093526298.445</v>
       </c>
       <c r="L41" s="5">
-        <f>K41-I41/X41</f>
+        <f t="shared" si="14"/>
         <v>46340093526054.031</v>
       </c>
       <c r="M41" s="1">
@@ -4331,11 +4331,11 @@
         <v>225.7</v>
       </c>
       <c r="P41" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.86907970735464002</v>
       </c>
       <c r="Q41" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>281.14728532922607</v>
       </c>
       <c r="R41" s="1">
@@ -4360,15 +4360,15 @@
         <v>6.9762399999999998</v>
       </c>
       <c r="Y41" s="2">
-        <f>E41/100*(J41/I41)</f>
+        <f t="shared" si="9"/>
         <v>0.40371919535511114</v>
       </c>
       <c r="Z41" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>29.39075742185209</v>
       </c>
       <c r="AA41" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1450.2747252747251</v>
       </c>
       <c r="AB41" s="4">
@@ -4383,26 +4383,26 @@
         <v>802.7</v>
       </c>
       <c r="C42" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.45375918598078013</v>
       </c>
       <c r="D42" s="3">
-        <f>Q42/I42</f>
+        <f t="shared" si="12"/>
         <v>0.17234050728837336</v>
       </c>
       <c r="E42" s="3">
         <v>62.9</v>
       </c>
       <c r="F42" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>37.1</v>
       </c>
       <c r="G42" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>954.822</v>
       </c>
       <c r="H42" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>563.178</v>
       </c>
       <c r="I42" s="3">
@@ -4415,7 +4415,7 @@
         <v>48438854527878.086</v>
       </c>
       <c r="L42" s="5">
-        <f>K42-I42/X42</f>
+        <f t="shared" si="14"/>
         <v>48438854527659.234</v>
       </c>
       <c r="M42" s="1">
@@ -4428,11 +4428,11 @@
         <v>248.6</v>
       </c>
       <c r="P42" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.8710581639803785</v>
       </c>
       <c r="Q42" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>304.87035739313245</v>
       </c>
       <c r="R42" s="1">
@@ -4457,15 +4457,15 @@
         <v>8.0831441666666706</v>
       </c>
       <c r="Y42" s="2">
-        <f>E42/100*(J42/I42)</f>
+        <f t="shared" si="9"/>
         <v>0.40481430186546075</v>
       </c>
       <c r="Z42" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>30.361072639909555</v>
       </c>
       <c r="AA42" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1518</v>
       </c>
       <c r="AB42" s="4">
@@ -4480,26 +4480,26 @@
         <v>804.5</v>
       </c>
       <c r="C43" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.4510540479928235</v>
       </c>
       <c r="D43" s="3">
-        <f>Q43/I43</f>
+        <f t="shared" si="12"/>
         <v>0.1677449755541362</v>
       </c>
       <c r="E43" s="3">
         <v>64</v>
       </c>
       <c r="F43" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>36</v>
       </c>
       <c r="G43" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>977.47724317295183</v>
       </c>
       <c r="H43" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>549.83094928478545</v>
       </c>
       <c r="I43" s="3">
@@ -4512,7 +4512,7 @@
         <v>49420951428837.398</v>
       </c>
       <c r="L43" s="5">
-        <f>K43-I43/X43</f>
+        <f t="shared" si="14"/>
         <v>49420951428623.094</v>
       </c>
       <c r="M43" s="1">
@@ -4525,11 +4525,11 @@
         <v>251</v>
       </c>
       <c r="P43" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.85900068446269684</v>
       </c>
       <c r="Q43" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>299.1899383983573</v>
       </c>
       <c r="R43" s="1">
@@ -4554,15 +4554,15 @@
         <v>8.3228174999999993</v>
       </c>
       <c r="Y43" s="2">
-        <f>E43/100*(J43/I43)</f>
+        <f t="shared" si="9"/>
         <v>0.42143978470509086</v>
       </c>
       <c r="Z43" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>32.408719443821489</v>
       </c>
       <c r="AA43" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1527.3081924577373</v>
       </c>
       <c r="AB43" s="4">
@@ -4577,26 +4577,26 @@
         <v>816.2</v>
       </c>
       <c r="C44" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.45549416820135052</v>
       </c>
       <c r="D44" s="3">
-        <f>Q44/I44</f>
+        <f t="shared" si="12"/>
         <v>0.16472797384788668</v>
       </c>
       <c r="E44" s="3">
         <v>64.7</v>
       </c>
       <c r="F44" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>35.299999999999997</v>
       </c>
       <c r="G44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>991.71041931384991</v>
       </c>
       <c r="H44" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>541.0722998729351</v>
       </c>
       <c r="I44" s="3">
@@ -4609,7 +4609,7 @@
         <v>50557000680031.789</v>
       </c>
       <c r="L44" s="5">
-        <f>K44-I44/X44</f>
+        <f t="shared" si="14"/>
         <v>50557000679804.812</v>
       </c>
       <c r="M44" s="1">
@@ -4622,11 +4622,11 @@
         <v>252.5</v>
       </c>
       <c r="P44" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.86739951906561308</v>
       </c>
       <c r="Q44" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>295.17605633802816</v>
       </c>
       <c r="R44" s="1">
@@ -4651,15 +4651,15 @@
         <v>7.8947141666666703</v>
       </c>
       <c r="Y44" s="2">
-        <f>E44/100*(J44/I44)</f>
+        <f t="shared" si="9"/>
         <v>0.43555784362966676</v>
       </c>
       <c r="Z44" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>34.278402293654779</v>
       </c>
       <c r="AA44" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1532.782719186785</v>
       </c>
       <c r="AB44" s="4">
@@ -4674,26 +4674,26 @@
         <v>827.1</v>
       </c>
       <c r="C45" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.45978097726388345</v>
       </c>
       <c r="D45" s="3">
-        <f>Q45/I45</f>
+        <f t="shared" si="12"/>
         <v>0.16790921284444801</v>
       </c>
       <c r="E45" s="3">
         <v>65.100000000000009</v>
       </c>
       <c r="F45" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>34.899999999999991</v>
       </c>
       <c r="G45" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1002.00225281602</v>
       </c>
       <c r="H45" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>537.17171464330386</v>
       </c>
       <c r="I45" s="3">
@@ -4706,7 +4706,7 @@
         <v>52127099001320.195</v>
       </c>
       <c r="L45" s="5">
-        <f>K45-I45/X45</f>
+        <f t="shared" si="14"/>
         <v>52127099001047.125</v>
       </c>
       <c r="M45" s="1">
@@ -4719,11 +4719,11 @@
         <v>259.7</v>
       </c>
       <c r="P45" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.87323470073974419</v>
       </c>
       <c r="Q45" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>302.05188298587757</v>
       </c>
       <c r="R45" s="1">
@@ -4748,15 +4748,15 @@
         <v>6.5876733333333304</v>
       </c>
       <c r="Y45" s="2">
-        <f>E45/100*(J45/I45)</f>
+        <f t="shared" si="9"/>
         <v>0.44504964144755133</v>
       </c>
       <c r="Z45" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>35.559466351659353</v>
       </c>
       <c r="AA45" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1539.1739674593239</v>
       </c>
       <c r="AB45" s="4">
@@ -4771,26 +4771,26 @@
         <v>865.5</v>
       </c>
       <c r="C46" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.46862309816449182</v>
       </c>
       <c r="D46" s="3">
-        <f>Q46/I46</f>
+        <f t="shared" si="12"/>
         <v>0.16735063312511025</v>
       </c>
       <c r="E46" s="3">
         <v>63.9</v>
       </c>
       <c r="F46" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>36.1</v>
       </c>
       <c r="G46" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1007.4246625766872</v>
       </c>
       <c r="H46" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>569.13975460122708</v>
       </c>
       <c r="I46" s="3">
@@ -4803,7 +4803,7 @@
         <v>54457959179311.562</v>
       </c>
       <c r="L46" s="5">
-        <f>K46-I46/X46</f>
+        <f t="shared" si="14"/>
         <v>54457959179003.289</v>
       </c>
       <c r="M46" s="1">
@@ -4816,11 +4816,11 @@
         <v>268.60000000000002</v>
       </c>
       <c r="P46" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.86311053984575847</v>
       </c>
       <c r="Q46" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>309.07988431876612</v>
       </c>
       <c r="R46" s="1">
@@ -4845,15 +4845,15 @@
         <v>5.9910566666666698</v>
       </c>
       <c r="Y46" s="2">
-        <f>E46/100*(J46/I46)</f>
+        <f t="shared" si="9"/>
         <v>0.44455633764686769</v>
       </c>
       <c r="Z46" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>36.231341518219715</v>
       </c>
       <c r="AA46" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1576.5644171779143</v>
       </c>
       <c r="AB46" s="4">
@@ -4868,26 +4868,26 @@
         <v>897.5</v>
       </c>
       <c r="C47" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.47486772486772488</v>
       </c>
       <c r="D47" s="3">
-        <f>Q47/I47</f>
+        <f t="shared" si="12"/>
         <v>0.17491584496944834</v>
       </c>
       <c r="E47" s="3">
         <v>64</v>
       </c>
       <c r="F47" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>36</v>
       </c>
       <c r="G47" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1026.0595947556615</v>
       </c>
       <c r="H47" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>577.15852205005956</v>
       </c>
       <c r="I47" s="3">
@@ -4900,7 +4900,7 @@
         <v>56639914120326.938</v>
       </c>
       <c r="L47" s="5">
-        <f>K47-I47/X47</f>
+        <f t="shared" si="14"/>
         <v>56639914120011.773</v>
       </c>
       <c r="M47" s="1">
@@ -4913,11 +4913,11 @@
         <v>292.60000000000002</v>
       </c>
       <c r="P47" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.87135199523525908</v>
       </c>
       <c r="Q47" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>330.59094699225739</v>
       </c>
       <c r="R47" s="1">
@@ -4942,15 +4942,15 @@
         <v>5.9969099999999997</v>
       </c>
       <c r="Y47" s="2">
-        <f>E47/100*(J47/I47)</f>
+        <f t="shared" si="9"/>
         <v>0.45548359788359782</v>
       </c>
       <c r="Z47" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>38.215073862433862</v>
       </c>
       <c r="AA47" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1603.2181168057211</v>
       </c>
       <c r="AB47" s="4">
@@ -4965,26 +4965,26 @@
         <v>924</v>
       </c>
       <c r="C48" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.47046843177189407</v>
       </c>
       <c r="D48" s="3">
-        <f>Q48/I48</f>
+        <f t="shared" si="12"/>
         <v>0.19184857446814046</v>
       </c>
       <c r="E48" s="3">
         <v>63.9</v>
       </c>
       <c r="F48" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>36.1</v>
       </c>
       <c r="G48" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1063.707584597433</v>
       </c>
       <c r="H48" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>600.93652275379225</v>
       </c>
       <c r="I48" s="3">
@@ -4997,7 +4997,7 @@
         <v>59154813079229.508</v>
       </c>
       <c r="L48" s="5">
-        <f>K48-I48/X48</f>
+        <f t="shared" si="14"/>
         <v>59154813078899.242</v>
       </c>
       <c r="M48" s="1">
@@ -5010,11 +5010,11 @@
         <v>342.1</v>
       </c>
       <c r="P48" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.87381864623243943</v>
       </c>
       <c r="Q48" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>376.79060025542788</v>
       </c>
       <c r="R48" s="1">
@@ -5039,15 +5039,15 @@
         <v>5.9467783333333299</v>
       </c>
       <c r="Y48" s="2">
-        <f>E48/100*(J48/I48)</f>
+        <f t="shared" si="9"/>
         <v>0.46415346232179222</v>
       </c>
       <c r="Z48" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>39.777951720977597</v>
       </c>
       <c r="AA48" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1664.6441073512251</v>
       </c>
       <c r="AB48" s="4">
@@ -5062,26 +5062,26 @@
         <v>940.30000000000018</v>
       </c>
       <c r="C49" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.47446765566656585</v>
       </c>
       <c r="D49" s="3">
-        <f>Q49/I49</f>
+        <f t="shared" si="12"/>
         <v>0.1907492690699846</v>
       </c>
       <c r="E49" s="3">
         <v>65.7</v>
       </c>
       <c r="F49" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>34.299999999999997</v>
       </c>
       <c r="G49" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1103.415393386545</v>
       </c>
       <c r="H49" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>576.06009122006833</v>
       </c>
       <c r="I49" s="3">
@@ -5094,7 +5094,7 @@
         <v>61743089955891.648</v>
       </c>
       <c r="L49" s="5">
-        <f>K49-I49/X49</f>
+        <f t="shared" si="14"/>
         <v>61743089955527.594</v>
       </c>
       <c r="M49" s="1">
@@ -5107,11 +5107,11 @@
         <v>356</v>
       </c>
       <c r="P49" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.87062851552946907</v>
       </c>
       <c r="Q49" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>378.02690144289545</v>
       </c>
       <c r="R49" s="1">
@@ -5136,15 +5136,15 @@
         <v>5.4437008333333301</v>
       </c>
       <c r="Y49" s="2">
-        <f>E49/100*(J49/I49)</f>
+        <f t="shared" si="9"/>
         <v>0.48829109900090834</v>
       </c>
       <c r="Z49" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>42.823129382379662</v>
       </c>
       <c r="AA49" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1679.4754846066135</v>
       </c>
       <c r="AB49" s="4">
@@ -5159,26 +5159,26 @@
         <v>944.90000000000009</v>
       </c>
       <c r="C50" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.47923112035299492</v>
       </c>
       <c r="D50" s="3">
-        <f>Q50/I50</f>
+        <f t="shared" si="12"/>
         <v>0.18668173527909643</v>
       </c>
       <c r="E50" s="3">
         <v>66</v>
       </c>
       <c r="F50" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>34</v>
       </c>
       <c r="G50" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1112.6849015317289</v>
       </c>
       <c r="H50" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>573.20131291028463</v>
       </c>
       <c r="I50" s="3">
@@ -5191,7 +5191,7 @@
         <v>63017282684022.266</v>
       </c>
       <c r="L50" s="5">
-        <f>K50-I50/X50</f>
+        <f t="shared" si="14"/>
         <v>63017282683635.516</v>
       </c>
       <c r="M50" s="1">
@@ -5204,11 +5204,11 @@
         <v>359.3</v>
       </c>
       <c r="P50" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.86934430195983547</v>
       </c>
       <c r="Q50" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>368.08037744979441</v>
       </c>
       <c r="R50" s="1">
@@ -5233,15 +5233,15 @@
         <v>5.0981308333333297</v>
       </c>
       <c r="Y50" s="2">
-        <f>E50/100*(J50/I50)</f>
+        <f t="shared" si="9"/>
         <v>0.51579550641578342</v>
       </c>
       <c r="Z50" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>47.143709286402611</v>
       </c>
       <c r="AA50" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1685.8862144420134</v>
       </c>
       <c r="AB50" s="4">
@@ -5256,26 +5256,26 @@
         <v>912.5</v>
       </c>
       <c r="C51" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.48669262360659232</v>
       </c>
       <c r="D51" s="3">
-        <f>Q51/I51</f>
+        <f t="shared" si="12"/>
         <v>0.16604075876080512</v>
       </c>
       <c r="E51" s="3">
         <v>68.3</v>
       </c>
       <c r="F51" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>31.700000000000003</v>
       </c>
       <c r="G51" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1102.4615886833512</v>
       </c>
       <c r="H51" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>511.6842219804135</v>
       </c>
       <c r="I51" s="3">
@@ -5288,7 +5288,7 @@
         <v>62157297842057.727</v>
       </c>
       <c r="L51" s="5">
-        <f>K51-I51/X51</f>
+        <f t="shared" si="14"/>
         <v>62157297841707.992</v>
       </c>
       <c r="M51" s="1">
@@ -5301,11 +5301,11 @@
         <v>293.40000000000009</v>
       </c>
       <c r="P51" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.84480276418082378</v>
       </c>
       <c r="Q51" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>311.30981860063355</v>
       </c>
       <c r="R51" s="1">
@@ -5330,15 +5330,15 @@
         <v>5.36086666666667</v>
       </c>
       <c r="Y51" s="2">
-        <f>E51/100*(J51/I51)</f>
+        <f t="shared" si="9"/>
         <v>0.540381993706331</v>
       </c>
       <c r="Z51" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>49.66110522161182</v>
       </c>
       <c r="AA51" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1614.1458106637649</v>
       </c>
       <c r="AB51" s="4">
@@ -5353,26 +5353,26 @@
         <v>919.6</v>
       </c>
       <c r="C52" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.48146596858638746</v>
       </c>
       <c r="D52" s="3">
-        <f>Q52/I52</f>
+        <f t="shared" si="12"/>
         <v>0.14879217213638105</v>
       </c>
       <c r="E52" s="3">
         <v>65.5</v>
       </c>
       <c r="F52" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>34.5</v>
       </c>
       <c r="G52" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1076.7426160337552</v>
       </c>
       <c r="H52" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>567.13924050632909</v>
       </c>
       <c r="I52" s="3">
@@ -5385,7 +5385,7 @@
         <v>64971660320224.367</v>
       </c>
       <c r="L52" s="5">
-        <f>K52-I52/X52</f>
+        <f t="shared" si="14"/>
         <v>64971660319884.758</v>
       </c>
       <c r="M52" s="1">
@@ -5398,11 +5398,11 @@
         <v>268.39999999999998</v>
       </c>
       <c r="P52" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.81829268292682922</v>
       </c>
       <c r="Q52" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>284.1930487804878</v>
       </c>
       <c r="R52" s="1">
@@ -5427,15 +5427,15 @@
         <v>5.6240750000000004</v>
       </c>
       <c r="Y52" s="2">
-        <f>E52/100*(J52/I52)</f>
+        <f t="shared" si="9"/>
         <v>0.53442513089005239</v>
       </c>
       <c r="Z52" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>50.663502408376971</v>
       </c>
       <c r="AA52" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1643.8818565400843</v>
       </c>
       <c r="AB52" s="4">
@@ -5450,26 +5450,26 @@
         <v>922.2</v>
       </c>
       <c r="C53" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.47646602944975464</v>
       </c>
       <c r="D53" s="3">
-        <f>Q53/I53</f>
+        <f t="shared" si="12"/>
         <v>0.14713693724585683</v>
       </c>
       <c r="E53" s="3">
         <v>65.100000000000009</v>
       </c>
       <c r="F53" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>34.899999999999991</v>
       </c>
       <c r="G53" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1084.2493710691826</v>
       </c>
       <c r="H53" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>581.2642557651991</v>
       </c>
       <c r="I53" s="3">
@@ -5482,7 +5482,7 @@
         <v>67126755546389.531</v>
       </c>
       <c r="L53" s="5">
-        <f>K53-I53/X53</f>
+        <f t="shared" si="14"/>
         <v>67126755546029.016</v>
       </c>
       <c r="M53" s="1">
@@ -5495,11 +5495,11 @@
         <v>274</v>
       </c>
       <c r="P53" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.81693500298151434</v>
       </c>
       <c r="Q53" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>284.78354203935589</v>
       </c>
       <c r="R53" s="1">
@@ -5524,15 +5524,15 @@
         <v>5.3687115350877201</v>
       </c>
       <c r="Y53" s="2">
-        <f>E53/100*(J53/I53)</f>
+        <f t="shared" si="9"/>
         <v>0.53442206148282112</v>
       </c>
       <c r="Z53" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>50.983864665461141</v>
       </c>
       <c r="AA53" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1665.5136268343817</v>
       </c>
       <c r="AB53" s="4">
@@ -5547,26 +5547,26 @@
         <v>926.90000000000009</v>
       </c>
       <c r="C54" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.4778081344399196</v>
       </c>
       <c r="D54" s="3">
-        <f>Q54/I54</f>
+        <f t="shared" si="12"/>
         <v>0.14878579677950868</v>
       </c>
       <c r="E54" s="3">
         <v>64.100000000000009</v>
       </c>
       <c r="F54" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>35.899999999999991</v>
       </c>
       <c r="G54" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1070.0172978505632</v>
       </c>
       <c r="H54" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>599.27645854657101</v>
       </c>
       <c r="I54" s="3">
@@ -5579,7 +5579,7 @@
         <v>68937636865008.312</v>
       </c>
       <c r="L54" s="5">
-        <f>K54-I54/X54</f>
+        <f t="shared" si="14"/>
         <v>68937636864673.414</v>
       </c>
       <c r="M54" s="1">
@@ -5592,11 +5592,11 @@
         <v>284</v>
       </c>
       <c r="P54" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.79820123664980325</v>
       </c>
       <c r="Q54" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>288.6295671725689</v>
       </c>
       <c r="R54" s="1">
@@ -5621,15 +5621,15 @@
         <v>5.7924755370391603</v>
       </c>
       <c r="Y54" s="2">
-        <f>E54/100*(J54/I54)</f>
+        <f t="shared" si="9"/>
         <v>0.53889731429455145</v>
       </c>
       <c r="Z54" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>52.650267606577678</v>
       </c>
       <c r="AA54" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1669.2937563971341</v>
       </c>
       <c r="AB54" s="4">
@@ -5644,26 +5644,26 @@
         <v>929.5</v>
       </c>
       <c r="C55" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.4747191011235955</v>
       </c>
       <c r="D55" s="3">
-        <f>Q55/I55</f>
+        <f t="shared" si="12"/>
         <v>0.15329467789854631</v>
       </c>
       <c r="E55" s="3">
         <v>64.100000000000009</v>
       </c>
       <c r="F55" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>35.899999999999991</v>
       </c>
       <c r="G55" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1078.1281947261664</v>
       </c>
       <c r="H55" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>603.81906693711949</v>
       </c>
       <c r="I55" s="3">
@@ -5676,7 +5676,7 @@
         <v>70867685078557.156</v>
       </c>
       <c r="L55" s="5">
-        <f>K55-I55/X55</f>
+        <f t="shared" si="14"/>
         <v>70867685078208.531</v>
       </c>
       <c r="M55" s="1">
@@ -5689,11 +5689,11 @@
         <v>297</v>
       </c>
       <c r="P55" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.80794341675734493</v>
       </c>
       <c r="Q55" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>300.15097932535366</v>
       </c>
       <c r="R55" s="1">
@@ -5718,15 +5718,15 @@
         <v>5.6163116861762203</v>
       </c>
       <c r="Y55" s="2">
-        <f>E55/100*(J55/I55)</f>
+        <f t="shared" si="9"/>
         <v>0.54291848825331979</v>
       </c>
       <c r="Z55" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>53.531762941777338</v>
       </c>
       <c r="AA55" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1681.9472616632859</v>
       </c>
       <c r="AB55" s="4">
@@ -5741,26 +5741,26 @@
         <v>938</v>
       </c>
       <c r="C56" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.47142785344524302</v>
       </c>
       <c r="D56" s="3">
-        <f>Q56/I56</f>
+        <f t="shared" si="12"/>
         <v>0.15374930166099421</v>
       </c>
       <c r="E56" s="3">
         <v>63.8</v>
       </c>
       <c r="F56" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>36.200000000000003</v>
       </c>
       <c r="G56" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1092.0945783132531</v>
       </c>
       <c r="H56" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>619.65240963855433</v>
       </c>
       <c r="I56" s="3">
@@ -5773,7 +5773,7 @@
         <v>73041202860769.609</v>
       </c>
       <c r="L56" s="5">
-        <f>K56-I56/X56</f>
+        <f t="shared" si="14"/>
         <v>73041202860415.094</v>
       </c>
       <c r="M56" s="1">
@@ -5786,11 +5786,11 @@
         <v>303.2</v>
       </c>
       <c r="P56" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.79852515143534364</v>
       </c>
       <c r="Q56" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>305.91498551488019</v>
       </c>
       <c r="R56" s="1">
@@ -5815,15 +5815,15 @@
         <v>5.6124666666666698</v>
       </c>
       <c r="Y56" s="2">
-        <f>E56/100*(J56/I56)</f>
+        <f t="shared" si="9"/>
         <v>0.54667849424536363</v>
       </c>
       <c r="Z56" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>54.449178026838226</v>
       </c>
       <c r="AA56" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1711.7469879518073</v>
       </c>
       <c r="AB56" s="4">
@@ -5838,26 +5838,26 @@
         <v>959.40000000000009</v>
       </c>
       <c r="C57" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.47112551561579258</v>
       </c>
       <c r="D57" s="3">
-        <f>Q57/I57</f>
+        <f t="shared" si="12"/>
         <v>0.16224710273030843</v>
       </c>
       <c r="E57" s="3">
         <v>64.100000000000009</v>
       </c>
       <c r="F57" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>35.899999999999991</v>
       </c>
       <c r="G57" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1121.4936000000002</v>
       </c>
       <c r="H57" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>628.10639999999989</v>
       </c>
       <c r="I57" s="3">
@@ -5870,7 +5870,7 @@
         <v>75283270551887.25</v>
       </c>
       <c r="L57" s="5">
-        <f>K57-I57/X57</f>
+        <f t="shared" si="14"/>
         <v>75283270551584.578</v>
       </c>
       <c r="M57" s="1">
@@ -5883,11 +5883,11 @@
         <v>330.40000000000009</v>
       </c>
       <c r="P57" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.81741712023750646</v>
       </c>
       <c r="Q57" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>330.40000000000009</v>
       </c>
       <c r="R57" s="1">
@@ -5912,15 +5912,15 @@
         <v>6.7279068312963002</v>
       </c>
       <c r="Y57" s="2">
-        <f>E57/100*(J57/I57)</f>
+        <f t="shared" si="9"/>
         <v>0.55072362993517976</v>
       </c>
       <c r="Z57" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>55.072362993517977</v>
       </c>
       <c r="AA57" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1749.6</v>
       </c>
       <c r="AB57" s="4">
@@ -5935,26 +5935,26 @@
         <v>982.6</v>
       </c>
       <c r="C58" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.46734839476813317</v>
       </c>
       <c r="D58" s="3">
-        <f>Q58/I58</f>
+        <f t="shared" si="12"/>
         <v>0.17020557441931347</v>
       </c>
       <c r="E58" s="3">
         <v>63.9</v>
       </c>
       <c r="F58" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>36.1</v>
       </c>
       <c r="G58" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1152.7483549351944</v>
       </c>
       <c r="H58" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>651.2396809571286</v>
       </c>
       <c r="I58" s="3">
@@ -5967,7 +5967,7 @@
         <v>77381232423345.172</v>
       </c>
       <c r="L58" s="5">
-        <f>K58-I58/X58</f>
+        <f t="shared" si="14"/>
         <v>77381232423032.844</v>
       </c>
       <c r="M58" s="1">
@@ -5980,11 +5980,11 @@
         <v>363.6</v>
       </c>
       <c r="P58" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.82039711191335751</v>
       </c>
       <c r="Q58" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>357.85722021660655</v>
       </c>
       <c r="R58" s="1">
@@ -6009,15 +6009,15 @@
         <v>6.7317182572463796</v>
       </c>
       <c r="Y58" s="2">
-        <f>E58/100*(J58/I58)</f>
+        <f t="shared" si="9"/>
         <v>0.54991990487514864</v>
       </c>
       <c r="Z58" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>55.156966458977408</v>
       </c>
       <c r="AA58" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1803.9880358923231</v>
       </c>
       <c r="AB58" s="4">
@@ -6032,26 +6032,26 @@
         <v>1005.1</v>
       </c>
       <c r="C59" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.4649366268850032</v>
       </c>
       <c r="D59" s="3">
-        <f>Q59/I59</f>
+        <f t="shared" si="12"/>
         <v>0.17632804703165866</v>
       </c>
       <c r="E59" s="3">
         <v>63.2</v>
       </c>
       <c r="F59" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>36.799999999999997</v>
       </c>
       <c r="G59" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1175.4950690335306</v>
       </c>
       <c r="H59" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>684.46548323471393</v>
       </c>
       <c r="I59" s="3">
@@ -6064,7 +6064,7 @@
         <v>80009142886740.656</v>
       </c>
       <c r="L59" s="5">
-        <f>K59-I59/X59</f>
+        <f t="shared" si="14"/>
         <v>80009142886413.25</v>
       </c>
       <c r="M59" s="1">
@@ -6077,11 +6077,11 @@
         <v>391.1</v>
       </c>
       <c r="P59" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.84017185821697105</v>
       </c>
       <c r="Q59" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>381.18597207303975</v>
       </c>
       <c r="R59" s="1">
@@ -6106,15 +6106,15 @@
         <v>6.6028934656140397</v>
       </c>
       <c r="Y59" s="2">
-        <f>E59/100*(J59/I59)</f>
+        <f t="shared" si="9"/>
         <v>0.5513701545008789</v>
       </c>
       <c r="Z59" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>55.908933666389125</v>
       </c>
       <c r="AA59" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1859.9605522682446</v>
       </c>
       <c r="AB59" s="4">
@@ -6129,26 +6129,26 @@
         <v>1040.2</v>
       </c>
       <c r="C60" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.471788824383164</v>
       </c>
       <c r="D60" s="3">
-        <f>Q60/I60</f>
+        <f t="shared" si="12"/>
         <v>0.18050799518222865</v>
       </c>
       <c r="E60" s="3">
         <v>63.6</v>
       </c>
       <c r="F60" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>36.4</v>
       </c>
       <c r="G60" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1203.6704500978472</v>
       </c>
       <c r="H60" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>688.89315068493136</v>
       </c>
       <c r="I60" s="3">
@@ -6161,7 +6161,7 @@
         <v>82630468929771.031</v>
       </c>
       <c r="L60" s="5">
-        <f>K60-I60/X60</f>
+        <f t="shared" si="14"/>
         <v>82630468929421.875</v>
       </c>
       <c r="M60" s="1">
@@ -6174,11 +6174,11 @@
         <v>412.3</v>
       </c>
       <c r="P60" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.84211601307189543</v>
       </c>
       <c r="Q60" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>397.98402777777778</v>
       </c>
       <c r="R60" s="1">
@@ -6203,15 +6203,15 @@
         <v>6.3146187866666699</v>
       </c>
       <c r="Y60" s="2">
-        <f>E60/100*(J60/I60)</f>
+        <f t="shared" si="9"/>
         <v>0.55794230769230768</v>
       </c>
       <c r="Z60" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>57.021703846153848</v>
       </c>
       <c r="AA60" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1892.5636007827786</v>
       </c>
       <c r="AB60" s="4">
@@ -6226,26 +6226,26 @@
         <v>1056.5999999999999</v>
       </c>
       <c r="C61" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.47218125754122536</v>
       </c>
       <c r="D61" s="3">
-        <f>Q61/I61</f>
+        <f t="shared" si="12"/>
         <v>0.17658908331298945</v>
       </c>
       <c r="E61" s="3">
         <v>64</v>
       </c>
       <c r="F61" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>36</v>
       </c>
       <c r="G61" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1231.1171345595353</v>
       </c>
       <c r="H61" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>692.50338818973864</v>
       </c>
       <c r="I61" s="3">
@@ -6258,7 +6258,7 @@
         <v>84771247102070.562</v>
       </c>
       <c r="L61" s="5">
-        <f>K61-I61/X61</f>
+        <f t="shared" si="14"/>
         <v>84771247101735.047</v>
       </c>
       <c r="M61" s="1">
@@ -6271,11 +6271,11 @@
         <v>416</v>
       </c>
       <c r="P61" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.84742310042778557</v>
       </c>
       <c r="Q61" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>395.15339172947643</v>
       </c>
       <c r="R61" s="1">
@@ -6300,15 +6300,15 @@
         <v>6.669446615</v>
       </c>
       <c r="Y61" s="2">
-        <f>E61/100*(J61/I61)</f>
+        <f t="shared" si="9"/>
         <v>0.56832640657818301</v>
       </c>
       <c r="Z61" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>58.708117799526306</v>
       </c>
       <c r="AA61" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1923.620522749274</v>
       </c>
       <c r="AB61" s="4">
@@ -6323,26 +6323,26 @@
         <v>1042.0999999999999</v>
       </c>
       <c r="C62" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.47726127776505606</v>
       </c>
       <c r="D62" s="3">
-        <f>Q62/I62</f>
+        <f t="shared" si="12"/>
         <v>0.18645987411730486</v>
       </c>
       <c r="E62" s="3">
         <v>63.7</v>
       </c>
       <c r="F62" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>36.299999999999997</v>
       </c>
       <c r="G62" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1215.932925682032</v>
       </c>
       <c r="H62" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>692.90997177798681</v>
       </c>
       <c r="I62" s="3">
@@ -6355,7 +6355,7 @@
         <v>82179103628835.375</v>
       </c>
       <c r="L62" s="5">
-        <f>K62-I62/X62</f>
+        <f t="shared" si="14"/>
         <v>82179103628501.609</v>
       </c>
       <c r="M62" s="1">
@@ -6368,11 +6368,11 @@
         <v>430.40000000000009</v>
       </c>
       <c r="P62" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.83686564262103835</v>
       </c>
       <c r="Q62" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>407.13513513513516</v>
       </c>
       <c r="R62" s="1">
@@ -6397,15 +6397,15 @@
         <v>6.54215220416667</v>
       </c>
       <c r="Y62" s="2">
-        <f>E62/100*(J62/I62)</f>
+        <f t="shared" si="9"/>
         <v>0.59195635447675754</v>
       </c>
       <c r="Z62" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>62.924960480879328</v>
       </c>
       <c r="AA62" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1908.8428974600188</v>
       </c>
       <c r="AB62" s="4">
@@ -6420,26 +6420,26 @@
         <v>1099.0999999999999</v>
       </c>
       <c r="C63" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.47113035277980192</v>
       </c>
       <c r="D63" s="3">
-        <f>Q63/I63</f>
+        <f t="shared" si="12"/>
         <v>0.1896265537459996</v>
       </c>
       <c r="E63" s="3">
         <v>61.4</v>
       </c>
       <c r="F63" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>38.6</v>
       </c>
       <c r="G63" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1248.1108874656909</v>
       </c>
       <c r="H63" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>784.64300091491327</v>
       </c>
       <c r="I63" s="3">
@@ -6452,7 +6452,7 @@
         <v>87297706317272.062</v>
       </c>
       <c r="L63" s="5">
-        <f>K63-I63/X63</f>
+        <f t="shared" si="14"/>
         <v>87297706316901</v>
       </c>
       <c r="M63" s="1">
@@ -6465,11 +6465,11 @@
         <v>481.2</v>
       </c>
       <c r="P63" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.85319148936170208</v>
       </c>
       <c r="Q63" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>442.37978723404251</v>
       </c>
       <c r="R63" s="1">
@@ -6494,15 +6494,15 @@
         <v>6.2871130825000003</v>
       </c>
       <c r="Y63" s="2">
-        <f>E63/100*(J63/I63)</f>
+        <f t="shared" si="9"/>
         <v>0.58475939817394662</v>
       </c>
       <c r="Z63" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>63.914202220412363</v>
       </c>
       <c r="AA63" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2032.7538883806042</v>
       </c>
       <c r="AB63" s="4">
@@ -6517,26 +6517,26 @@
         <v>1083.4000000000001</v>
       </c>
       <c r="C64" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.4520570808645582</v>
       </c>
       <c r="D64" s="3">
-        <f>Q64/I64</f>
+        <f t="shared" si="12"/>
         <v>0.19146585017533779</v>
       </c>
       <c r="E64" s="3">
         <v>59.1</v>
       </c>
       <c r="F64" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>40.9</v>
       </c>
       <c r="G64" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1234.2499999999998</v>
       </c>
       <c r="H64" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>854.15947546531288</v>
       </c>
       <c r="I64" s="3">
@@ -6549,7 +6549,7 @@
         <v>89994663432855.266</v>
       </c>
       <c r="L64" s="5">
-        <f>K64-I64/X64</f>
+        <f t="shared" si="14"/>
         <v>89994663432516.578</v>
       </c>
       <c r="M64" s="1">
@@ -6562,11 +6562,11 @@
         <v>527.80000000000007</v>
       </c>
       <c r="P64" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0.85737491877842764</v>
       </c>
       <c r="Q64" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>458.86705653021454</v>
       </c>
       <c r="R64" s="1">
@@ -6591,15 +6591,15 @@
         <v>7.0761518624999997</v>
       </c>
       <c r="Y64" s="2">
-        <f>E64/100*(J64/I64)</f>
+        <f t="shared" si="9"/>
         <v>0.60873049319869821</v>
       </c>
       <c r="Z64" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>71.951944296086126</v>
       </c>
       <c r="AA64" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2088.4094754653129</v>
       </c>
       <c r="AB64" s="4">

</xml_diff>